<commit_message>
Removing Extra Vide Code
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/Frames/Test/Frames for P4.xlsx
+++ b/Dataset Excel Sheets/Frames/Test/Frames for P4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salma\Desktop\Senior Design\CSE 491 - Senior Design II\github\Senior-Design-Code\Dataset Excel Sheets\Frames\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC9A7BB-BEBF-4D95-9B8F-F3ED3E12F03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CD4FB3-59CE-4E53-8785-057BBF195268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>count</t>
   </si>
@@ -43,26 +43,32 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>2: [2, 2]</t>
+    <t>No overlap between 2 &amp; 3</t>
   </si>
   <si>
-    <t>3: [3, 3]</t>
+    <t>No overlap between 3 &amp; 4</t>
   </si>
   <si>
-    <t>4: [4, 4]</t>
+    <t>2: [68, 85.75]</t>
   </si>
   <si>
-    <t>5: [5, 5]</t>
+    <t>3: [102.5, 128.75]</t>
   </si>
   <si>
-    <t>No overlap between anything</t>
+    <t>4: [130.25, 165]</t>
+  </si>
+  <si>
+    <t>5: [151.25, 173]</t>
+  </si>
+  <si>
+    <t>Small overlap between 4 &amp; 5 (13.75 frames)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +80,21 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -97,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -117,6 +138,19 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -244,43 +278,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,19 +618,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q115"/>
+  <dimension ref="A1:N115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>2</v>
       </c>
@@ -609,1324 +648,1322 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>129</v>
+      </c>
+      <c r="C2">
+        <v>129</v>
+      </c>
+      <c r="D2">
+        <v>168</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="H2" s="7">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="I2" s="7">
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="J2" s="8">
         <v>5</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4">
+      <c r="L2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+      <c r="C3">
+        <v>114</v>
+      </c>
+      <c r="D3">
+        <v>161</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>114</v>
+      </c>
+      <c r="H3" s="5">
+        <v>90</v>
+      </c>
+      <c r="I3" s="5">
+        <v>54</v>
+      </c>
+      <c r="J3" s="10">
+        <v>50</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>126</v>
+      </c>
+      <c r="C4">
+        <v>115</v>
+      </c>
+      <c r="D4">
+        <v>136</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>80.017544000000001</v>
+      </c>
+      <c r="H4" s="5">
+        <v>117.744444</v>
+      </c>
+      <c r="I4" s="5">
+        <v>146.81481500000001</v>
+      </c>
+      <c r="J4" s="10">
+        <v>162.22</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>77</v>
+      </c>
+      <c r="B5">
+        <v>136</v>
+      </c>
+      <c r="C5">
+        <v>131</v>
+      </c>
+      <c r="D5">
+        <v>171</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4">
+      <c r="G5" s="5">
+        <v>18.747499000000001</v>
+      </c>
+      <c r="H5" s="5">
+        <v>20.547321</v>
+      </c>
+      <c r="I5" s="5">
+        <v>24.778317999999999</v>
+      </c>
+      <c r="J5" s="10">
+        <v>21.993774999999999</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="3"/>
+      <c r="N5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>133</v>
+      </c>
+      <c r="C6">
+        <v>118</v>
+      </c>
+      <c r="D6">
+        <v>146</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4">
+      <c r="G6" s="5">
+        <v>48</v>
+      </c>
+      <c r="H6" s="5">
+        <v>73</v>
+      </c>
+      <c r="I6" s="5">
+        <v>94</v>
+      </c>
+      <c r="J6" s="10">
+        <v>78</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>65</v>
+      </c>
+      <c r="B7">
+        <v>131</v>
+      </c>
+      <c r="C7">
+        <v>135</v>
+      </c>
+      <c r="D7">
+        <v>151</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="5">
+        <v>68</v>
+      </c>
+      <c r="H7" s="5">
+        <v>102.5</v>
+      </c>
+      <c r="I7" s="5">
+        <v>130.25</v>
+      </c>
+      <c r="J7" s="10">
+        <v>151.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>52</v>
+      </c>
+      <c r="B8">
+        <v>120</v>
+      </c>
+      <c r="C8">
+        <v>139</v>
+      </c>
+      <c r="D8">
+        <v>194</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>75.5</v>
+      </c>
+      <c r="H8" s="5">
+        <v>116</v>
+      </c>
+      <c r="I8" s="5">
+        <v>147.5</v>
+      </c>
+      <c r="J8" s="10">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>54</v>
+      </c>
+      <c r="B9">
+        <v>110</v>
+      </c>
+      <c r="C9">
+        <v>146</v>
+      </c>
+      <c r="D9">
+        <v>184</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="G9" s="5">
+        <v>85.75</v>
+      </c>
+      <c r="H9" s="5">
+        <v>128.75</v>
+      </c>
+      <c r="I9" s="5">
+        <v>165</v>
+      </c>
+      <c r="J9" s="10">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>106</v>
+      </c>
+      <c r="C10">
+        <v>160</v>
+      </c>
+      <c r="D10">
+        <v>134</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5">
-        <v>5</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>114</v>
-      </c>
-      <c r="H3" s="2">
-        <v>90</v>
-      </c>
-      <c r="I3" s="2">
-        <v>54</v>
-      </c>
-      <c r="J3" s="7">
-        <v>50</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2">
-        <v>4</v>
-      </c>
-      <c r="J4" s="7">
-        <v>5</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2">
-        <v>2</v>
-      </c>
-      <c r="H6" s="2">
-        <v>3</v>
-      </c>
-      <c r="I6" s="2">
-        <v>4</v>
-      </c>
-      <c r="J6" s="7">
-        <v>5</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2">
-        <v>3</v>
-      </c>
-      <c r="I7" s="2">
-        <v>4</v>
-      </c>
-      <c r="J7" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2</v>
-      </c>
-      <c r="H8" s="2">
-        <v>3</v>
-      </c>
-      <c r="I8" s="2">
-        <v>4</v>
-      </c>
-      <c r="J8" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2">
-        <v>3</v>
-      </c>
-      <c r="I9" s="2">
-        <v>4</v>
-      </c>
-      <c r="J9" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="10">
-        <v>2</v>
-      </c>
-      <c r="H10" s="10">
-        <v>3</v>
-      </c>
-      <c r="I10" s="10">
-        <v>4</v>
-      </c>
-      <c r="J10" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G10" s="13">
+        <v>127</v>
+      </c>
+      <c r="H10" s="13">
+        <v>189</v>
+      </c>
+      <c r="I10" s="13">
+        <v>203</v>
+      </c>
+      <c r="J10" s="14">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>148</v>
       </c>
       <c r="D11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>168</v>
       </c>
       <c r="D12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>188</v>
       </c>
       <c r="D13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>147</v>
       </c>
       <c r="D14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>123</v>
       </c>
       <c r="D15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>121</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>131</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>158</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>170</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>137</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>171</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>141</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>178</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>184</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>152</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>147</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>203</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>179</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>125</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>153</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>168</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>156</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>165</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="D35">
-        <v>5</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>172</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>2</v>
+        <v>64</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>113</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>150</v>
       </c>
       <c r="D38">
-        <v>5</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>127</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>128</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>141</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="B43">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>141</v>
       </c>
       <c r="D43">
-        <v>5</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="B44">
-        <v>3</v>
+        <v>115</v>
       </c>
       <c r="C44">
-        <v>4</v>
+        <v>187</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>157</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="B46">
-        <v>3</v>
+        <v>122</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>165</v>
       </c>
       <c r="D46">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>2</v>
+        <v>93</v>
       </c>
       <c r="B47">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>138</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>172</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>148</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>2</v>
+        <v>126</v>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="C50">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="D50">
-        <v>5</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="C51">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>155</v>
       </c>
       <c r="C52">
-        <v>4</v>
+        <v>95</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="C53">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>189</v>
       </c>
       <c r="C54">
-        <v>4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>160</v>
       </c>
       <c r="C55">
-        <v>4</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="B57">
-        <v>3</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="B59">
-        <v>3</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B60">
-        <v>3</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>2</v>
+        <v>114</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="B71">
-        <v>3</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="B72">
-        <v>3</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="B73">
-        <v>3</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B74">
-        <v>3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>2</v>
+        <v>79</v>
       </c>
       <c r="B75">
-        <v>3</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="B76">
-        <v>3</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="B78">
-        <v>3</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="B80">
-        <v>3</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="B81">
-        <v>3</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>2</v>
+        <v>83</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B83">
-        <v>3</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="B85">
-        <v>3</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>2</v>
+        <v>127</v>
       </c>
       <c r="B87">
-        <v>3</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>2</v>
+        <v>112</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>124</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>2</v>
+        <v>115</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="B91">
-        <v>3</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>2</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>2</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>2</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>2</v>
+        <v>76</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>2</v>
+        <v>67</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>2</v>
+        <v>65</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>2</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>2</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>2</v>
+        <v>64</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>2</v>
+        <v>75</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>2</v>
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>2</v>
+        <v>61</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>2</v>
+        <v>71</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>2</v>
+        <v>91</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>2</v>
+        <v>80</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>2</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>